<commit_message>
doc(rapport plan de test)
</commit_message>
<xml_diff>
--- a/Doc/CI-CD-Journal-de-Travail_NademoYosef.xlsx
+++ b/Doc/CI-CD-Journal-de-Travail_NademoYosef.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\cicd-todo-app\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD992A6-1FF6-468B-B303-6A5021D89003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0D1D81-EA2C-420F-A905-BDFE35489076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="7215" yWindow="420" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>Auteur:</t>
   </si>
@@ -159,6 +159,15 @@
   <si>
     <t>conéxion SSH</t>
   </si>
+  <si>
+    <t>workflow travail chez-moi</t>
+  </si>
+  <si>
+    <t>workflow pour le backend</t>
+  </si>
+  <si>
+    <t>workflow pour le frontend</t>
+  </si>
 </sst>
 </file>
 
@@ -171,7 +180,7 @@
     <numFmt numFmtId="167" formatCode="dd\ mmm"/>
     <numFmt numFmtId="168" formatCode="00\ &quot;min&quot;"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -295,8 +304,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -375,8 +391,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -423,12 +445,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF9D9FAC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9D9FAC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -635,6 +668,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1182,7 +1218,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2112,16 +2148,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.19047619047619047</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2857142857142857</c:v>
+                  <c:v>0.53125</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.52380952380952384</c:v>
+                  <c:v>0.34375</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4310,7 +4346,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4365,7 +4401,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>1 heures 45 minutes</v>
+        <v>2 heures 40 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4384,11 +4420,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>105</v>
+        <v>160</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>105</v>
+        <v>160</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4590,16 +4626,26 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="63" t="str">
+      <c r="A13" s="63">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="34"/>
+        <v>49</v>
+      </c>
+      <c r="B13" s="89">
+        <v>45992</v>
+      </c>
       <c r="C13" s="35"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="84"/>
+      <c r="D13" s="36">
+        <v>30</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="84" t="s">
+        <v>39</v>
+      </c>
       <c r="N13">
         <v>6</v>
       </c>
@@ -4608,15 +4654,23 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="62" t="str">
+      <c r="A14" s="62">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="30"/>
+        <v>49</v>
+      </c>
+      <c r="B14" s="30">
+        <v>45992</v>
+      </c>
       <c r="C14" s="31"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="23"/>
+      <c r="D14" s="32">
+        <v>25</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>41</v>
+      </c>
       <c r="G14" s="39"/>
       <c r="N14">
         <v>7</v>
@@ -11025,7 +11079,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.19047619047619047</v>
+        <v>0.125</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11046,11 +11100,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11058,11 +11112,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>0 h 30 min</v>
+        <v>1 h 25 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.2857142857142857</v>
+        <v>0.53125</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11136,7 +11190,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.52380952380952384</v>
+        <v>0.34375</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11192,22 +11246,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>105</v>
+        <v>160</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>105</v>
+        <v>160</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 45 min</v>
+        <v>2 h 40 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>7.2916666666666671E-2</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11251,15 +11305,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11268,6 +11313,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11472,14 +11526,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11488,6 +11534,14 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>